<commit_message>
add my Rproj back in and some other files
</commit_message>
<xml_diff>
--- a/CAMS/SMB_FY2019_discRd_BG_example.xlsx
+++ b/CAMS/SMB_FY2019_discRd_BG_example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="mack" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="catch" sheetId="5" r:id="rId5"/>
     <sheet name="summary" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet2" sheetId="8" r:id="rId8"/>
+    <sheet name="ACL CAMS compare" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -724,15 +724,15 @@
       <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -758,7 +758,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -781,7 +781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -804,7 +804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -830,7 +830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -856,7 +856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -882,7 +882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -908,7 +908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -934,7 +934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -960,7 +960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -986,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>6.6287993710171964</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>81446701.866338253</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>1824.7154300329271</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>223.75221846819571</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>110.2248865819265</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>10.88872554504216</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>36</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>109891057.79252972</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>39</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>4299</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>0.51264732791561285</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>3.8994014388944409</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>23.56468386024325</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>5.1088032127543244</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>10.96258570208175</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>9.40119536796553E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -2645,14 +2645,14 @@
       <selection activeCell="H33" sqref="A30:H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2955,7 +2955,7 @@
         <v>9.7482343691429367</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>1268.7146403800959</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -3330,7 +3330,7 @@
         <v>3465.0059578611422</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>368.28223164100888</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>15.294568251128579</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>36521.08572088433</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>9847.9744198464668</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>81724.414944276039</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -3624,7 +3624,7 @@
         <v>10809.813445344131</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -3673,7 +3673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -3803,7 +3803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -4002,7 +4002,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -4129,7 +4129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -4175,7 +4175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>5.519902519026682E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>3.4022762654040702E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -4417,7 +4417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -4495,7 +4495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -4531,19 +4531,19 @@
   <dimension ref="A1:H75"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="768" topLeftCell="A2"/>
+      <pane ySplit="765" topLeftCell="A2"/>
       <selection activeCell="F1" sqref="F1:G1048576"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -4592,7 +4592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -4641,7 +4641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -4719,7 +4719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -4846,7 +4846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -4898,7 +4898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -4947,7 +4947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -5045,7 +5045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -5097,7 +5097,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -5123,7 +5123,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -5198,7 +5198,7 @@
         <v>269.76299052139251</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>1173.5819359937409</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -5244,7 +5244,7 @@
         <v>381.35264397224</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -5267,7 +5267,7 @@
         <v>109.8103843983635</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>36</v>
       </c>
@@ -5293,7 +5293,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
@@ -5319,7 +5319,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>39</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -5397,7 +5397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -5446,7 +5446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -5469,7 +5469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -5567,7 +5567,7 @@
         <v>402.42815241375598</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -5619,7 +5619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -5645,7 +5645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -5772,7 +5772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -5821,7 +5821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -5844,7 +5844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -5870,7 +5870,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -5922,7 +5922,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -5948,7 +5948,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -5971,7 +5971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -5997,7 +5997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -6046,7 +6046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -6069,7 +6069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -6092,7 +6092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -6115,7 +6115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -6141,7 +6141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -6193,7 +6193,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -6219,7 +6219,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -6242,7 +6242,7 @@
         <v>1.8399675063422279E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -6265,7 +6265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -6288,7 +6288,7 @@
         <v>2.1220275097995311</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -6311,7 +6311,7 @@
         <v>0.46577595243128161</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -6337,7 +6337,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -6363,7 +6363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -6389,7 +6389,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -6428,13 +6428,13 @@
       <selection activeCell="F1" sqref="F1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6460,7 +6460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -6483,7 +6483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -6506,7 +6506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -6532,7 +6532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -6558,7 +6558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -6584,7 +6584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -6610,7 +6610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -6636,7 +6636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -6688,7 +6688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -6737,7 +6737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -6763,7 +6763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -6789,7 +6789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -6812,7 +6812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -6838,7 +6838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -6861,7 +6861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -6887,7 +6887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -6913,7 +6913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -6936,7 +6936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -6962,7 +6962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -6988,7 +6988,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -7014,7 +7014,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -7040,7 +7040,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -7066,7 +7066,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -7089,7 +7089,7 @@
         <v>1960.1727230031829</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -7112,7 +7112,7 @@
         <v>1879.479684520212</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -7135,7 +7135,7 @@
         <v>2737.4563230780609</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -7158,7 +7158,7 @@
         <v>386.66514796748942</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -7184,7 +7184,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -7210,7 +7210,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -7236,7 +7236,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -7262,7 +7262,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -7288,7 +7288,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -7314,7 +7314,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -7337,7 +7337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -7360,7 +7360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -7386,7 +7386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -7409,7 +7409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -7458,7 +7458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -7484,7 +7484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -7510,7 +7510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -7536,7 +7536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -7588,7 +7588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -7614,7 +7614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -7640,7 +7640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -7663,7 +7663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -7686,7 +7686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -7712,7 +7712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -7735,7 +7735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -7761,7 +7761,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -7787,7 +7787,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -7813,7 +7813,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -7839,7 +7839,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -7862,7 +7862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -7888,7 +7888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -7914,7 +7914,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -7937,7 +7937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -7960,7 +7960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -7983,7 +7983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -8006,7 +8006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -8032,7 +8032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -8058,7 +8058,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -8084,7 +8084,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -8110,7 +8110,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -8133,7 +8133,7 @@
         <v>9.1998375317111376E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -8156,7 +8156,7 @@
         <v>0.1465212026018109</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -8179,7 +8179,7 @@
         <v>0.2789866537631337</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -8202,7 +8202,7 @@
         <v>2.1695066233766609E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -8228,7 +8228,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -8254,7 +8254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -8280,7 +8280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -8317,9 +8317,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>82</v>
       </c>
@@ -8330,7 +8330,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -8341,7 +8341,7 @@
         <v>137813</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -8352,7 +8352,7 @@
         <v>95068</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -8363,7 +8363,7 @@
         <v>186489</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -8387,16 +8387,16 @@
       <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>82</v>
       </c>
@@ -8416,7 +8416,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -8436,7 +8436,7 @@
         <v>4803.696062957024</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -8456,7 +8456,7 @@
         <v>5269.5290770444872</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -8476,7 +8476,7 @@
         <v>12853.130391994249</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -8509,18 +8509,18 @@
       <selection activeCell="I14" sqref="A1:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>97</v>
       </c>
@@ -8549,7 +8549,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>93</v>
       </c>
@@ -8575,7 +8575,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>94</v>
       </c>
@@ -8601,7 +8601,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>95</v>
       </c>
@@ -8627,11 +8627,11 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -8660,7 +8660,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>39</v>
       </c>
@@ -8686,7 +8686,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>36</v>
       </c>
@@ -8712,7 +8712,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>38</v>
       </c>
@@ -8738,11 +8738,11 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>99</v>
       </c>
@@ -8778,7 +8778,7 @@
         <v>-0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12">
         <f t="shared" ref="C12:I14" si="1">C7-C2</f>
         <v>610</v>
@@ -8808,7 +8808,7 @@
         <v>-0.25999999999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C13">
         <f t="shared" si="1"/>
         <v>468</v>
@@ -8838,7 +8838,7 @@
         <v>-1.0000000000000009E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14">
         <f t="shared" si="1"/>
         <v>621</v>
@@ -8868,7 +8868,7 @@
         <v>-9.9999999999998979E-3</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>97</v>
       </c>
@@ -8876,7 +8876,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>5</v>
       </c>
@@ -8887,7 +8887,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>92</v>
       </c>
@@ -8905,7 +8905,7 @@
         <v>3833376.1368651316</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>93</v>
       </c>
@@ -8923,7 +8923,7 @@
         <v>3250841.3018146493</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>94</v>
       </c>
@@ -8941,7 +8941,7 @@
         <v>1236899.9738707989</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>95</v>
       </c>
@@ -8973,14 +8973,14 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>82</v>
       </c>
@@ -8991,7 +8991,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -9002,7 +9002,7 @@
         <v>3840933</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -9013,7 +9013,7 @@
         <v>274320</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -9024,7 +9024,7 @@
         <v>676245</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -9035,25 +9035,25 @@
         <v>2915101</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>

</xml_diff>